<commit_message>
Version 1.1 with TAC functionality
</commit_message>
<xml_diff>
--- a/output/LORELEI_0147_2000_1023_Gold_3-13-21.xlsx
+++ b/output/LORELEI_0147_2000_1023_Gold_3-13-21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daniel/Desktop/AutoAspect/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1792D8-DA48-CD43-A473-26BEFE9042C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB5315-D53E-3B41-B97F-04AFEA87C93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="500" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
     <col min="4" max="4" width="15.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="3"/>
+    <col min="7" max="7" width="13.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.2">

</xml_diff>